<commit_message>
New Template changes - UD
</commit_message>
<xml_diff>
--- a/src/EPR.Calculator.Frontend/wwwroot/assets/SchemeParameterTemplates/SchemeParameterTemplate.v0.1.xlsx
+++ b/src/EPR.Calculator.Frontend/wwwroot/assets/SchemeParameterTemplates/SchemeParameterTemplate.v0.1.xlsx
@@ -1,15 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27914"/>
-  <fileSharing readOnlyRecommended="1"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28005"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eviden-my.sharepoint.com/personal/chris_m_bush_eviden_com/Documents/DEFRA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37F97659-029E-45B1-A310-73A56BE4ED17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CBA5ACF9-C9BF-4591-8C3F-D3824D50C444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{774E54A3-E1B1-4BB4-866A-0176C4ECA77D}"/>
   </bookViews>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="79">
   <si>
     <t>Parameter Unique Ref</t>
   </si>
@@ -69,7 +68,7 @@
     <t>Aluminium</t>
   </si>
   <si>
-    <t>1. Update Parameter_Values</t>
+    <t>1. Update the values in column F: 'Parameter Value'</t>
   </si>
   <si>
     <t>COMC-FC</t>
@@ -78,7 +77,7 @@
     <t>Fibre composite</t>
   </si>
   <si>
-    <t>2. File</t>
+    <t>2. Select 'File' menu</t>
   </si>
   <si>
     <t>COMC-GL</t>
@@ -87,7 +86,7 @@
     <t>Glass</t>
   </si>
   <si>
-    <t>3. Save a Copy</t>
+    <t>3. Select 'Save a Copy' option</t>
   </si>
   <si>
     <t>COMC-PC</t>
@@ -96,7 +95,7 @@
     <t>Paper or card</t>
   </si>
   <si>
-    <t>4. Save as type:  CSV UTF-8 (Comma delimited) (*.csv)</t>
+    <t>4. Select file type:  CSV UTF-8 (Comma delimited) (*.csv)</t>
   </si>
   <si>
     <t>COMC-PL</t>
@@ -132,81 +131,48 @@
     <t>England</t>
   </si>
   <si>
-    <t>https://www.gov.uk/government/publications/packaging-data-how-to-create-your-file-for-extended-producer-responsibility/packaging-data-file-specification-for-extended-producer-responsibility#packaging-material-codes</t>
-  </si>
-  <si>
     <t>SAOC-WLS</t>
   </si>
   <si>
     <t>Wales</t>
   </si>
   <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>SAOC-SCT</t>
   </si>
   <si>
     <t>Scotland</t>
   </si>
   <si>
-    <t>AL</t>
-  </si>
-  <si>
     <t>SAOC-NIR</t>
   </si>
   <si>
     <t>Northern Ireland</t>
   </si>
   <si>
-    <t>FC</t>
-  </si>
-  <si>
     <t>LAPC-ENG</t>
   </si>
   <si>
     <t>Local authority data preparation costs</t>
   </si>
   <si>
-    <t>GL</t>
-  </si>
-  <si>
     <t>LAPC-WLS</t>
   </si>
   <si>
-    <t>PC</t>
-  </si>
-  <si>
     <t>LAPC-SCT</t>
   </si>
   <si>
-    <t>PL</t>
-  </si>
-  <si>
     <t>LAPC-NIR</t>
   </si>
   <si>
-    <t>ST</t>
-  </si>
-  <si>
     <t>SCSC-ENG</t>
   </si>
   <si>
     <t>Scheme setup costs</t>
   </si>
   <si>
-    <t>WD</t>
-  </si>
-  <si>
     <t>SCSC-WLS</t>
   </si>
   <si>
-    <t>OT</t>
-  </si>
-  <si>
     <t>SCSC-SCT</t>
   </si>
   <si>
@@ -222,36 +188,21 @@
     <t>LRET-FC</t>
   </si>
   <si>
-    <t>Use consistent country codes - GOV.UK (www.gov.uk)</t>
-  </si>
-  <si>
     <t>LRET-GL</t>
   </si>
   <si>
     <t>LRET-PC</t>
   </si>
   <si>
-    <t>ENG</t>
-  </si>
-  <si>
     <t>LRET-PL</t>
   </si>
   <si>
-    <t>WLS</t>
-  </si>
-  <si>
     <t>LRET-ST</t>
   </si>
   <si>
-    <t>SCT</t>
-  </si>
-  <si>
     <t>LRET-WD</t>
   </si>
   <si>
-    <t>NIR</t>
-  </si>
-  <si>
     <t>LRET-OT</t>
   </si>
   <si>
@@ -297,7 +248,7 @@
     <t>Tonnage change threshold</t>
   </si>
   <si>
-    <t>TONT-DI</t>
+    <t>TONT-AD</t>
   </si>
   <si>
     <t>TONT-PI</t>
@@ -334,7 +285,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -371,14 +322,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -386,7 +329,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -395,19 +338,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFE1F5FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -458,74 +389,63 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="8" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="8" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="8" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -846,29 +766,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43329FAA-6043-4598-BAD3-349FEDFA5DF0}">
-  <dimension ref="A1:I91"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" style="17" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" style="13" customWidth="1"/>
     <col min="2" max="2" width="34.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="16" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="12" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="49.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="51.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="4"/>
     <col min="9" max="9" width="14.85546875" style="4" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -890,8 +810,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:7">
+      <c r="A2" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -903,18 +823,18 @@
       <c r="D2" s="5">
         <v>0</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="17">
         <v>999999999.99000001</v>
       </c>
       <c r="F2" s="6">
         <v>2210.4499999999998</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:7">
+      <c r="A3" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -926,18 +846,18 @@
       <c r="D3" s="5">
         <v>0</v>
       </c>
-      <c r="E3" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F3" s="8">
+      <c r="E3" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F3" s="7">
         <v>2210</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="17" t="s">
+    <row r="4" spans="1:7">
+      <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -949,18 +869,18 @@
       <c r="D4" s="5">
         <v>0</v>
       </c>
-      <c r="E4" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F4" s="8">
+      <c r="E4" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F4" s="7">
         <v>2210</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="17" t="s">
+    <row r="5" spans="1:7">
+      <c r="A5" s="13" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -972,18 +892,18 @@
       <c r="D5" s="5">
         <v>0</v>
       </c>
-      <c r="E5" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F5" s="8">
+      <c r="E5" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F5" s="7">
         <v>2210</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="17" t="s">
+    <row r="6" spans="1:7">
+      <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -995,15 +915,15 @@
       <c r="D6" s="5">
         <v>0</v>
       </c>
-      <c r="E6" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F6" s="8">
+      <c r="E6" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F6" s="7">
         <v>2210</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="17" t="s">
+    <row r="7" spans="1:7">
+      <c r="A7" s="13" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1015,15 +935,15 @@
       <c r="D7" s="5">
         <v>0</v>
       </c>
-      <c r="E7" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F7" s="8">
+      <c r="E7" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F7" s="7">
         <v>2210</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="17" t="s">
+    <row r="8" spans="1:7">
+      <c r="A8" s="13" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -1035,15 +955,15 @@
       <c r="D8" s="5">
         <v>0</v>
       </c>
-      <c r="E8" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F8" s="8">
+      <c r="E8" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F8" s="7">
         <v>2210</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="17" t="s">
+    <row r="9" spans="1:7">
+      <c r="A9" s="13" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1055,17 +975,15 @@
       <c r="D9" s="5">
         <v>0</v>
       </c>
-      <c r="E9" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F9" s="8">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="17" t="s">
+      <c r="E9" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="13" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -1077,100 +995,79 @@
       <c r="D10" s="5">
         <v>0</v>
       </c>
-      <c r="E10" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F10" s="8">
+      <c r="E10" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F10" s="7">
         <v>500</v>
       </c>
-      <c r="H10" s="20" t="s">
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="13" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="17" t="s">
-        <v>32</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F11" s="7">
+        <v>140.55000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="13" t="s">
         <v>33</v>
-      </c>
-      <c r="D11" s="5">
-        <v>0</v>
-      </c>
-      <c r="E11" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F11" s="8">
-        <v>140.55000000000001</v>
-      </c>
-      <c r="H11" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="17" t="s">
-        <v>36</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D12" s="5">
         <v>0</v>
       </c>
-      <c r="E12" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F12" s="8">
+      <c r="E12" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F12" s="7">
         <v>170</v>
       </c>
-      <c r="H12" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="17" t="s">
-        <v>39</v>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="13" t="s">
+        <v>35</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D13" s="5">
         <v>0</v>
       </c>
-      <c r="E13" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F13" s="8">
+      <c r="E13" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F13" s="7">
         <v>90</v>
       </c>
-      <c r="H13" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="17" t="s">
-        <v>42</v>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>30</v>
@@ -1178,103 +1075,79 @@
       <c r="D14" s="5">
         <v>0</v>
       </c>
-      <c r="E14" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F14" s="8">
+      <c r="E14" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F14" s="7">
         <v>115.45</v>
       </c>
-      <c r="H14" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="17" t="s">
-        <v>45</v>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0</v>
+      </c>
+      <c r="E15" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F15" s="7">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0</v>
+      </c>
+      <c r="E16" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F16" s="7">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0</v>
+      </c>
+      <c r="E17" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F17" s="7">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="5">
-        <v>0</v>
-      </c>
-      <c r="E15" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F15" s="8">
-        <v>114</v>
-      </c>
-      <c r="H15" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="5">
-        <v>0</v>
-      </c>
-      <c r="E16" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F16" s="8">
-        <v>117</v>
-      </c>
-      <c r="H16" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="5">
-        <v>0</v>
-      </c>
-      <c r="E17" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F17" s="8">
-        <v>19</v>
-      </c>
-      <c r="H17" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>30</v>
@@ -1282,543 +1155,498 @@
       <c r="D18" s="5">
         <v>0</v>
       </c>
-      <c r="E18" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F18" s="8">
+      <c r="E18" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F18" s="7">
         <v>325.55</v>
       </c>
-      <c r="H18" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="17" t="s">
-        <v>54</v>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D19" s="5">
         <v>0</v>
       </c>
-      <c r="E19" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F19" s="8">
+      <c r="E19" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F19" s="7">
         <v>314</v>
       </c>
-      <c r="H19" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="17" t="s">
-        <v>56</v>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D20" s="5">
         <v>0</v>
       </c>
-      <c r="E20" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F20" s="8">
+      <c r="E20" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F20" s="7">
         <v>317</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="17" t="s">
-        <v>57</v>
+    <row r="21" spans="1:6">
+      <c r="A21" s="13" t="s">
+        <v>46</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D21" s="5">
         <v>0</v>
       </c>
-      <c r="E21" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F21" s="8">
+      <c r="E21" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F21" s="7">
         <v>391.09899999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="17" t="s">
-        <v>58</v>
+    <row r="22" spans="1:6">
+      <c r="A22" s="13" t="s">
+        <v>47</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="9">
-        <v>0</v>
-      </c>
-      <c r="E22" s="10">
-        <v>999999999</v>
-      </c>
-      <c r="F22" s="11">
+      <c r="D22" s="8">
+        <v>0</v>
+      </c>
+      <c r="E22" s="9">
+        <v>999999999.99899995</v>
+      </c>
+      <c r="F22" s="10">
         <v>70.55</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="17" t="s">
+    <row r="23" spans="1:6">
+      <c r="A23" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="8">
+        <v>0</v>
+      </c>
+      <c r="E23" s="9">
+        <v>999999999.99899995</v>
+      </c>
+      <c r="F23" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="8">
+        <v>0</v>
+      </c>
+      <c r="E24" s="9">
+        <v>999999999.99899995</v>
+      </c>
+      <c r="F24" s="10">
         <v>60</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="9">
-        <v>0</v>
-      </c>
-      <c r="E23" s="10">
-        <v>999999999</v>
-      </c>
-      <c r="F23" s="11">
-        <v>80</v>
-      </c>
-      <c r="H23" s="24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" s="4" t="s">
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="8">
+        <v>0</v>
+      </c>
+      <c r="E25" s="9">
+        <v>999999999.99899995</v>
+      </c>
+      <c r="F25" s="10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="9">
-        <v>0</v>
-      </c>
-      <c r="E24" s="10">
-        <v>999999999</v>
-      </c>
-      <c r="F24" s="11">
-        <v>60</v>
-      </c>
-      <c r="H24" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" s="4" t="s">
+      <c r="D26" s="8">
+        <v>0</v>
+      </c>
+      <c r="E26" s="9">
+        <v>999999999.99899995</v>
+      </c>
+      <c r="F26" s="10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="9">
-        <v>0</v>
-      </c>
-      <c r="E25" s="10">
-        <v>999999999</v>
-      </c>
-      <c r="F25" s="11">
-        <v>50</v>
-      </c>
-      <c r="H25" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="I25" s="4" t="s">
+      <c r="D27" s="8">
+        <v>0</v>
+      </c>
+      <c r="E27" s="9">
+        <v>999999999.99899995</v>
+      </c>
+      <c r="F27" s="10">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="4" t="s">
+    <row r="28" spans="1:6">
+      <c r="A28" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="9">
-        <v>0</v>
-      </c>
-      <c r="E26" s="10">
-        <v>999999999</v>
-      </c>
-      <c r="F26" s="11">
-        <v>40</v>
-      </c>
-      <c r="H26" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="9">
-        <v>0</v>
-      </c>
-      <c r="E27" s="10">
-        <v>999999999</v>
-      </c>
-      <c r="F27" s="11">
-        <v>30</v>
-      </c>
-      <c r="H27" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" s="9">
-        <v>0</v>
-      </c>
-      <c r="E28" s="10">
-        <v>999999999</v>
-      </c>
-      <c r="F28" s="11">
-        <v>20</v>
-      </c>
-      <c r="H28" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="17" t="s">
-        <v>71</v>
+      <c r="D28" s="8">
+        <v>0</v>
+      </c>
+      <c r="E28" s="9">
+        <v>999999999.99899995</v>
+      </c>
+      <c r="F28" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="13" t="s">
+        <v>55</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="9">
-        <v>0</v>
-      </c>
-      <c r="E29" s="10">
-        <v>999999999</v>
-      </c>
-      <c r="F29" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="17" t="s">
-        <v>72</v>
+      <c r="D29" s="8">
+        <v>0</v>
+      </c>
+      <c r="E29" s="9">
+        <v>999999999.99899995</v>
+      </c>
+      <c r="F29" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="13" t="s">
+        <v>56</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D30" s="12">
-        <v>0</v>
-      </c>
-      <c r="E30" s="12">
-        <v>1000</v>
+        <v>58</v>
+      </c>
+      <c r="D30" s="11">
+        <v>0</v>
+      </c>
+      <c r="E30" s="11">
+        <v>9.9999000000000002</v>
       </c>
       <c r="F30" s="2">
-        <v>5.2499999999999998E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="B31" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="C31" s="21" t="s">
-        <v>77</v>
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="D31" s="5">
         <v>0</v>
       </c>
-      <c r="E31" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F31" s="8">
+      <c r="E31" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F31" s="7">
         <v>5000</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="B32" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="C32" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D32" s="5">
-        <v>0</v>
-      </c>
-      <c r="E32" s="5">
+    <row r="32" spans="1:6">
+      <c r="A32" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="17">
         <v>-999999999.99000001</v>
       </c>
-      <c r="F32" s="8">
+      <c r="E32" s="17">
+        <v>0</v>
+      </c>
+      <c r="F32" s="7">
         <v>-1000</v>
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="B33" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="C33" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D33" s="12">
-        <v>0</v>
-      </c>
-      <c r="E33" s="12">
-        <v>10</v>
+      <c r="A33" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="11">
+        <v>0</v>
+      </c>
+      <c r="E33" s="11">
+        <v>9.9999000000000002</v>
       </c>
       <c r="F33" s="2">
         <v>0.02</v>
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="B34" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="D34" s="12">
-        <v>0</v>
-      </c>
-      <c r="E34" s="18">
-        <v>-10</v>
+      <c r="A34" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" s="11">
+        <v>-9.9999000000000002</v>
+      </c>
+      <c r="E34" s="11">
+        <v>0</v>
       </c>
       <c r="F34" s="2">
         <v>-0.01</v>
       </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="B35" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C35" s="21" t="s">
-        <v>77</v>
+      <c r="A35" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="D35" s="5">
         <v>0</v>
       </c>
-      <c r="E35" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F35" s="8">
+      <c r="E35" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F35" s="7">
         <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="B36" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C36" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D36" s="5">
-        <v>0</v>
-      </c>
-      <c r="E36" s="5">
+      <c r="A36" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36" s="17">
         <v>-999999999.99000001</v>
       </c>
-      <c r="F36" s="8">
+      <c r="E36" s="17">
+        <v>0</v>
+      </c>
+      <c r="F36" s="7">
         <v>-10</v>
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="B37" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C37" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D37" s="12">
-        <v>0</v>
-      </c>
-      <c r="E37" s="12">
-        <v>10</v>
+      <c r="A37" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37" s="11">
+        <v>0</v>
+      </c>
+      <c r="E37" s="11">
+        <v>9.9999000000000002</v>
       </c>
       <c r="F37" s="2">
         <v>0.02</v>
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="B38" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C38" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="D38" s="12">
-        <v>0</v>
-      </c>
-      <c r="E38" s="18">
-        <v>-10</v>
+      <c r="A38" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D38" s="11">
+        <v>-9.9999000000000002</v>
+      </c>
+      <c r="E38" s="11">
+        <v>0</v>
       </c>
       <c r="F38" s="2">
         <v>-5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C39" s="7" t="s">
+      <c r="A39" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D39" s="13">
-        <v>0</v>
-      </c>
-      <c r="E39" s="13">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F39" s="14">
+      <c r="D39" s="5">
+        <v>0</v>
+      </c>
+      <c r="E39" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F39" s="7">
         <v>115.45</v>
       </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D40" s="13">
-        <v>0</v>
-      </c>
-      <c r="E40" s="13">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F40" s="14">
+      <c r="A40" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D40" s="5">
+        <v>0</v>
+      </c>
+      <c r="E40" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F40" s="7">
         <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D41" s="13">
-        <v>0</v>
-      </c>
-      <c r="E41" s="13">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F41" s="14">
+      <c r="A41" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41" s="5">
+        <v>0</v>
+      </c>
+      <c r="E41" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F41" s="7">
         <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D42" s="13">
-        <v>0</v>
-      </c>
-      <c r="E42" s="13">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F42" s="15">
+      <c r="A42" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D42" s="5">
+        <v>0</v>
+      </c>
+      <c r="E42" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F42" s="18">
         <v>19</v>
       </c>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="B43" s="22"/>
+      <c r="A43" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" s="15"/>
     </row>
     <row r="50" spans="4:5">
       <c r="D50" s="3"/>
@@ -1829,20 +1657,20 @@
       <c r="E51" s="5"/>
     </row>
     <row r="52" spans="4:5">
-      <c r="D52" s="9"/>
-      <c r="E52" s="10"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="9"/>
     </row>
     <row r="53" spans="4:5">
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
     </row>
     <row r="54" spans="4:5">
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
     </row>
     <row r="55" spans="4:5">
-      <c r="D55" s="12"/>
-      <c r="E55" s="18"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="14"/>
     </row>
     <row r="56" spans="4:5">
       <c r="D56" s="4"/>
@@ -1989,22 +1817,14 @@
       <c r="E91" s="4"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="H23" r:id="rId1" xr:uid="{B5EB0F45-ED5D-4DE6-9BA1-6FE6BBDD9003}"/>
-    <hyperlink ref="H10" r:id="rId2" location="packaging-material-codes" xr:uid="{6ECCDCF6-D832-47BD-BFFE-6CACBA086DC3}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="d1117845-93f6-4da3-abaa-fcb4fa669c78" ContentTypeId="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC01" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2013,7 +1833,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lae2bfa7b6474897ab4a53f76ea236c7 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
@@ -2078,7 +1898,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Defra document" ma:contentTypeID="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC01004F33776538BC6A4BB35A13B55FDEF669" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="540aecd89ea7381fdbb9d30c8a4dc936">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="662745e8-e224-48e8-a2e3-254862b8c2f5" xmlns:ns3="aa328a9d-dd77-40c9-a5eb-135ff6df47d2" xmlns:ns4="afded164-4d4a-45c5-b6a4-4c86a507a889" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f33d7f383e7ef3e5f94429c699357eeb" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2433,18 +2253,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="d1117845-93f6-4da3-abaa-fcb4fa669c78" ContentTypeId="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC01" PreviousValue="false"/>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FC065CC-1BDB-4473-8699-DD8F45A40C86}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B31069A-A18C-4C15-8712-D6A4154B76E5}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B31069A-A18C-4C15-8712-D6A4154B76E5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74398F8A-5630-46AB-8D4D-D0AED34105A4}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74398F8A-5630-46AB-8D4D-D0AED34105A4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F008D6C-356D-4A95-A106-F742FD21AA0E}"/>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F008D6C-356D-4A95-A106-F742FD21AA0E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FC065CC-1BDB-4473-8699-DD8F45A40C86}"/>
 </file>
</xml_diff>

<commit_message>
New Template changes - UD (#23)
</commit_message>
<xml_diff>
--- a/src/EPR.Calculator.Frontend/wwwroot/assets/SchemeParameterTemplates/SchemeParameterTemplate.v0.1.xlsx
+++ b/src/EPR.Calculator.Frontend/wwwroot/assets/SchemeParameterTemplates/SchemeParameterTemplate.v0.1.xlsx
@@ -1,15 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27914"/>
-  <fileSharing readOnlyRecommended="1"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28005"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eviden-my.sharepoint.com/personal/chris_m_bush_eviden_com/Documents/DEFRA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37F97659-029E-45B1-A310-73A56BE4ED17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CBA5ACF9-C9BF-4591-8C3F-D3824D50C444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{774E54A3-E1B1-4BB4-866A-0176C4ECA77D}"/>
   </bookViews>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="79">
   <si>
     <t>Parameter Unique Ref</t>
   </si>
@@ -69,7 +68,7 @@
     <t>Aluminium</t>
   </si>
   <si>
-    <t>1. Update Parameter_Values</t>
+    <t>1. Update the values in column F: 'Parameter Value'</t>
   </si>
   <si>
     <t>COMC-FC</t>
@@ -78,7 +77,7 @@
     <t>Fibre composite</t>
   </si>
   <si>
-    <t>2. File</t>
+    <t>2. Select 'File' menu</t>
   </si>
   <si>
     <t>COMC-GL</t>
@@ -87,7 +86,7 @@
     <t>Glass</t>
   </si>
   <si>
-    <t>3. Save a Copy</t>
+    <t>3. Select 'Save a Copy' option</t>
   </si>
   <si>
     <t>COMC-PC</t>
@@ -96,7 +95,7 @@
     <t>Paper or card</t>
   </si>
   <si>
-    <t>4. Save as type:  CSV UTF-8 (Comma delimited) (*.csv)</t>
+    <t>4. Select file type:  CSV UTF-8 (Comma delimited) (*.csv)</t>
   </si>
   <si>
     <t>COMC-PL</t>
@@ -132,81 +131,48 @@
     <t>England</t>
   </si>
   <si>
-    <t>https://www.gov.uk/government/publications/packaging-data-how-to-create-your-file-for-extended-producer-responsibility/packaging-data-file-specification-for-extended-producer-responsibility#packaging-material-codes</t>
-  </si>
-  <si>
     <t>SAOC-WLS</t>
   </si>
   <si>
     <t>Wales</t>
   </si>
   <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>SAOC-SCT</t>
   </si>
   <si>
     <t>Scotland</t>
   </si>
   <si>
-    <t>AL</t>
-  </si>
-  <si>
     <t>SAOC-NIR</t>
   </si>
   <si>
     <t>Northern Ireland</t>
   </si>
   <si>
-    <t>FC</t>
-  </si>
-  <si>
     <t>LAPC-ENG</t>
   </si>
   <si>
     <t>Local authority data preparation costs</t>
   </si>
   <si>
-    <t>GL</t>
-  </si>
-  <si>
     <t>LAPC-WLS</t>
   </si>
   <si>
-    <t>PC</t>
-  </si>
-  <si>
     <t>LAPC-SCT</t>
   </si>
   <si>
-    <t>PL</t>
-  </si>
-  <si>
     <t>LAPC-NIR</t>
   </si>
   <si>
-    <t>ST</t>
-  </si>
-  <si>
     <t>SCSC-ENG</t>
   </si>
   <si>
     <t>Scheme setup costs</t>
   </si>
   <si>
-    <t>WD</t>
-  </si>
-  <si>
     <t>SCSC-WLS</t>
   </si>
   <si>
-    <t>OT</t>
-  </si>
-  <si>
     <t>SCSC-SCT</t>
   </si>
   <si>
@@ -222,36 +188,21 @@
     <t>LRET-FC</t>
   </si>
   <si>
-    <t>Use consistent country codes - GOV.UK (www.gov.uk)</t>
-  </si>
-  <si>
     <t>LRET-GL</t>
   </si>
   <si>
     <t>LRET-PC</t>
   </si>
   <si>
-    <t>ENG</t>
-  </si>
-  <si>
     <t>LRET-PL</t>
   </si>
   <si>
-    <t>WLS</t>
-  </si>
-  <si>
     <t>LRET-ST</t>
   </si>
   <si>
-    <t>SCT</t>
-  </si>
-  <si>
     <t>LRET-WD</t>
   </si>
   <si>
-    <t>NIR</t>
-  </si>
-  <si>
     <t>LRET-OT</t>
   </si>
   <si>
@@ -297,7 +248,7 @@
     <t>Tonnage change threshold</t>
   </si>
   <si>
-    <t>TONT-DI</t>
+    <t>TONT-AD</t>
   </si>
   <si>
     <t>TONT-PI</t>
@@ -334,7 +285,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -371,14 +322,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -386,7 +329,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -395,19 +338,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFE1F5FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -458,74 +389,63 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="8" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="8" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="8" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -846,29 +766,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43329FAA-6043-4598-BAD3-349FEDFA5DF0}">
-  <dimension ref="A1:I91"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" style="17" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" style="13" customWidth="1"/>
     <col min="2" max="2" width="34.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="16" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="12" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="49.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="51.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="4"/>
     <col min="9" max="9" width="14.85546875" style="4" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -890,8 +810,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:7">
+      <c r="A2" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -903,18 +823,18 @@
       <c r="D2" s="5">
         <v>0</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="17">
         <v>999999999.99000001</v>
       </c>
       <c r="F2" s="6">
         <v>2210.4499999999998</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:7">
+      <c r="A3" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -926,18 +846,18 @@
       <c r="D3" s="5">
         <v>0</v>
       </c>
-      <c r="E3" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F3" s="8">
+      <c r="E3" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F3" s="7">
         <v>2210</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="17" t="s">
+    <row r="4" spans="1:7">
+      <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -949,18 +869,18 @@
       <c r="D4" s="5">
         <v>0</v>
       </c>
-      <c r="E4" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F4" s="8">
+      <c r="E4" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F4" s="7">
         <v>2210</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="17" t="s">
+    <row r="5" spans="1:7">
+      <c r="A5" s="13" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -972,18 +892,18 @@
       <c r="D5" s="5">
         <v>0</v>
       </c>
-      <c r="E5" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F5" s="8">
+      <c r="E5" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F5" s="7">
         <v>2210</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="17" t="s">
+    <row r="6" spans="1:7">
+      <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -995,15 +915,15 @@
       <c r="D6" s="5">
         <v>0</v>
       </c>
-      <c r="E6" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F6" s="8">
+      <c r="E6" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F6" s="7">
         <v>2210</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="17" t="s">
+    <row r="7" spans="1:7">
+      <c r="A7" s="13" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1015,15 +935,15 @@
       <c r="D7" s="5">
         <v>0</v>
       </c>
-      <c r="E7" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F7" s="8">
+      <c r="E7" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F7" s="7">
         <v>2210</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="17" t="s">
+    <row r="8" spans="1:7">
+      <c r="A8" s="13" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -1035,15 +955,15 @@
       <c r="D8" s="5">
         <v>0</v>
       </c>
-      <c r="E8" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F8" s="8">
+      <c r="E8" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F8" s="7">
         <v>2210</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="17" t="s">
+    <row r="9" spans="1:7">
+      <c r="A9" s="13" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1055,17 +975,15 @@
       <c r="D9" s="5">
         <v>0</v>
       </c>
-      <c r="E9" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F9" s="8">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="17" t="s">
+      <c r="E9" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="13" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -1077,100 +995,79 @@
       <c r="D10" s="5">
         <v>0</v>
       </c>
-      <c r="E10" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F10" s="8">
+      <c r="E10" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F10" s="7">
         <v>500</v>
       </c>
-      <c r="H10" s="20" t="s">
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="13" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="17" t="s">
-        <v>32</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F11" s="7">
+        <v>140.55000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="13" t="s">
         <v>33</v>
-      </c>
-      <c r="D11" s="5">
-        <v>0</v>
-      </c>
-      <c r="E11" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F11" s="8">
-        <v>140.55000000000001</v>
-      </c>
-      <c r="H11" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="17" t="s">
-        <v>36</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D12" s="5">
         <v>0</v>
       </c>
-      <c r="E12" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F12" s="8">
+      <c r="E12" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F12" s="7">
         <v>170</v>
       </c>
-      <c r="H12" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="17" t="s">
-        <v>39</v>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="13" t="s">
+        <v>35</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D13" s="5">
         <v>0</v>
       </c>
-      <c r="E13" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F13" s="8">
+      <c r="E13" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F13" s="7">
         <v>90</v>
       </c>
-      <c r="H13" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="17" t="s">
-        <v>42</v>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>30</v>
@@ -1178,103 +1075,79 @@
       <c r="D14" s="5">
         <v>0</v>
       </c>
-      <c r="E14" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F14" s="8">
+      <c r="E14" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F14" s="7">
         <v>115.45</v>
       </c>
-      <c r="H14" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="17" t="s">
-        <v>45</v>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0</v>
+      </c>
+      <c r="E15" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F15" s="7">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0</v>
+      </c>
+      <c r="E16" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F16" s="7">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0</v>
+      </c>
+      <c r="E17" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F17" s="7">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="5">
-        <v>0</v>
-      </c>
-      <c r="E15" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F15" s="8">
-        <v>114</v>
-      </c>
-      <c r="H15" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="5">
-        <v>0</v>
-      </c>
-      <c r="E16" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F16" s="8">
-        <v>117</v>
-      </c>
-      <c r="H16" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="5">
-        <v>0</v>
-      </c>
-      <c r="E17" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F17" s="8">
-        <v>19</v>
-      </c>
-      <c r="H17" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>30</v>
@@ -1282,543 +1155,498 @@
       <c r="D18" s="5">
         <v>0</v>
       </c>
-      <c r="E18" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F18" s="8">
+      <c r="E18" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F18" s="7">
         <v>325.55</v>
       </c>
-      <c r="H18" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="17" t="s">
-        <v>54</v>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D19" s="5">
         <v>0</v>
       </c>
-      <c r="E19" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F19" s="8">
+      <c r="E19" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F19" s="7">
         <v>314</v>
       </c>
-      <c r="H19" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="17" t="s">
-        <v>56</v>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D20" s="5">
         <v>0</v>
       </c>
-      <c r="E20" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F20" s="8">
+      <c r="E20" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F20" s="7">
         <v>317</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="17" t="s">
-        <v>57</v>
+    <row r="21" spans="1:6">
+      <c r="A21" s="13" t="s">
+        <v>46</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D21" s="5">
         <v>0</v>
       </c>
-      <c r="E21" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F21" s="8">
+      <c r="E21" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F21" s="7">
         <v>391.09899999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="17" t="s">
-        <v>58</v>
+    <row r="22" spans="1:6">
+      <c r="A22" s="13" t="s">
+        <v>47</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="9">
-        <v>0</v>
-      </c>
-      <c r="E22" s="10">
-        <v>999999999</v>
-      </c>
-      <c r="F22" s="11">
+      <c r="D22" s="8">
+        <v>0</v>
+      </c>
+      <c r="E22" s="9">
+        <v>999999999.99899995</v>
+      </c>
+      <c r="F22" s="10">
         <v>70.55</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="17" t="s">
+    <row r="23" spans="1:6">
+      <c r="A23" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="8">
+        <v>0</v>
+      </c>
+      <c r="E23" s="9">
+        <v>999999999.99899995</v>
+      </c>
+      <c r="F23" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="8">
+        <v>0</v>
+      </c>
+      <c r="E24" s="9">
+        <v>999999999.99899995</v>
+      </c>
+      <c r="F24" s="10">
         <v>60</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="9">
-        <v>0</v>
-      </c>
-      <c r="E23" s="10">
-        <v>999999999</v>
-      </c>
-      <c r="F23" s="11">
-        <v>80</v>
-      </c>
-      <c r="H23" s="24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" s="4" t="s">
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="8">
+        <v>0</v>
+      </c>
+      <c r="E25" s="9">
+        <v>999999999.99899995</v>
+      </c>
+      <c r="F25" s="10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="9">
-        <v>0</v>
-      </c>
-      <c r="E24" s="10">
-        <v>999999999</v>
-      </c>
-      <c r="F24" s="11">
-        <v>60</v>
-      </c>
-      <c r="H24" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" s="4" t="s">
+      <c r="D26" s="8">
+        <v>0</v>
+      </c>
+      <c r="E26" s="9">
+        <v>999999999.99899995</v>
+      </c>
+      <c r="F26" s="10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="9">
-        <v>0</v>
-      </c>
-      <c r="E25" s="10">
-        <v>999999999</v>
-      </c>
-      <c r="F25" s="11">
-        <v>50</v>
-      </c>
-      <c r="H25" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="I25" s="4" t="s">
+      <c r="D27" s="8">
+        <v>0</v>
+      </c>
+      <c r="E27" s="9">
+        <v>999999999.99899995</v>
+      </c>
+      <c r="F27" s="10">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="4" t="s">
+    <row r="28" spans="1:6">
+      <c r="A28" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="9">
-        <v>0</v>
-      </c>
-      <c r="E26" s="10">
-        <v>999999999</v>
-      </c>
-      <c r="F26" s="11">
-        <v>40</v>
-      </c>
-      <c r="H26" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="9">
-        <v>0</v>
-      </c>
-      <c r="E27" s="10">
-        <v>999999999</v>
-      </c>
-      <c r="F27" s="11">
-        <v>30</v>
-      </c>
-      <c r="H27" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" s="9">
-        <v>0</v>
-      </c>
-      <c r="E28" s="10">
-        <v>999999999</v>
-      </c>
-      <c r="F28" s="11">
-        <v>20</v>
-      </c>
-      <c r="H28" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="17" t="s">
-        <v>71</v>
+      <c r="D28" s="8">
+        <v>0</v>
+      </c>
+      <c r="E28" s="9">
+        <v>999999999.99899995</v>
+      </c>
+      <c r="F28" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="13" t="s">
+        <v>55</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="9">
-        <v>0</v>
-      </c>
-      <c r="E29" s="10">
-        <v>999999999</v>
-      </c>
-      <c r="F29" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="17" t="s">
-        <v>72</v>
+      <c r="D29" s="8">
+        <v>0</v>
+      </c>
+      <c r="E29" s="9">
+        <v>999999999.99899995</v>
+      </c>
+      <c r="F29" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="13" t="s">
+        <v>56</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D30" s="12">
-        <v>0</v>
-      </c>
-      <c r="E30" s="12">
-        <v>1000</v>
+        <v>58</v>
+      </c>
+      <c r="D30" s="11">
+        <v>0</v>
+      </c>
+      <c r="E30" s="11">
+        <v>9.9999000000000002</v>
       </c>
       <c r="F30" s="2">
-        <v>5.2499999999999998E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="B31" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="C31" s="21" t="s">
-        <v>77</v>
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="D31" s="5">
         <v>0</v>
       </c>
-      <c r="E31" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F31" s="8">
+      <c r="E31" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F31" s="7">
         <v>5000</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="B32" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="C32" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D32" s="5">
-        <v>0</v>
-      </c>
-      <c r="E32" s="5">
+    <row r="32" spans="1:6">
+      <c r="A32" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="17">
         <v>-999999999.99000001</v>
       </c>
-      <c r="F32" s="8">
+      <c r="E32" s="17">
+        <v>0</v>
+      </c>
+      <c r="F32" s="7">
         <v>-1000</v>
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="B33" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="C33" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D33" s="12">
-        <v>0</v>
-      </c>
-      <c r="E33" s="12">
-        <v>10</v>
+      <c r="A33" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="11">
+        <v>0</v>
+      </c>
+      <c r="E33" s="11">
+        <v>9.9999000000000002</v>
       </c>
       <c r="F33" s="2">
         <v>0.02</v>
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="B34" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="D34" s="12">
-        <v>0</v>
-      </c>
-      <c r="E34" s="18">
-        <v>-10</v>
+      <c r="A34" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" s="11">
+        <v>-9.9999000000000002</v>
+      </c>
+      <c r="E34" s="11">
+        <v>0</v>
       </c>
       <c r="F34" s="2">
         <v>-0.01</v>
       </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="B35" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C35" s="21" t="s">
-        <v>77</v>
+      <c r="A35" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="D35" s="5">
         <v>0</v>
       </c>
-      <c r="E35" s="5">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F35" s="8">
+      <c r="E35" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F35" s="7">
         <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="B36" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C36" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D36" s="5">
-        <v>0</v>
-      </c>
-      <c r="E36" s="5">
+      <c r="A36" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36" s="17">
         <v>-999999999.99000001</v>
       </c>
-      <c r="F36" s="8">
+      <c r="E36" s="17">
+        <v>0</v>
+      </c>
+      <c r="F36" s="7">
         <v>-10</v>
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="B37" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C37" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D37" s="12">
-        <v>0</v>
-      </c>
-      <c r="E37" s="12">
-        <v>10</v>
+      <c r="A37" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37" s="11">
+        <v>0</v>
+      </c>
+      <c r="E37" s="11">
+        <v>9.9999000000000002</v>
       </c>
       <c r="F37" s="2">
         <v>0.02</v>
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="B38" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C38" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="D38" s="12">
-        <v>0</v>
-      </c>
-      <c r="E38" s="18">
-        <v>-10</v>
+      <c r="A38" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D38" s="11">
+        <v>-9.9999000000000002</v>
+      </c>
+      <c r="E38" s="11">
+        <v>0</v>
       </c>
       <c r="F38" s="2">
         <v>-5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C39" s="7" t="s">
+      <c r="A39" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D39" s="13">
-        <v>0</v>
-      </c>
-      <c r="E39" s="13">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F39" s="14">
+      <c r="D39" s="5">
+        <v>0</v>
+      </c>
+      <c r="E39" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F39" s="7">
         <v>115.45</v>
       </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D40" s="13">
-        <v>0</v>
-      </c>
-      <c r="E40" s="13">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F40" s="14">
+      <c r="A40" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D40" s="5">
+        <v>0</v>
+      </c>
+      <c r="E40" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F40" s="7">
         <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D41" s="13">
-        <v>0</v>
-      </c>
-      <c r="E41" s="13">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F41" s="14">
+      <c r="A41" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41" s="5">
+        <v>0</v>
+      </c>
+      <c r="E41" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F41" s="7">
         <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D42" s="13">
-        <v>0</v>
-      </c>
-      <c r="E42" s="13">
-        <v>999999999.99000001</v>
-      </c>
-      <c r="F42" s="15">
+      <c r="A42" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D42" s="5">
+        <v>0</v>
+      </c>
+      <c r="E42" s="17">
+        <v>999999999.99000001</v>
+      </c>
+      <c r="F42" s="18">
         <v>19</v>
       </c>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="B43" s="22"/>
+      <c r="A43" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" s="15"/>
     </row>
     <row r="50" spans="4:5">
       <c r="D50" s="3"/>
@@ -1829,20 +1657,20 @@
       <c r="E51" s="5"/>
     </row>
     <row r="52" spans="4:5">
-      <c r="D52" s="9"/>
-      <c r="E52" s="10"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="9"/>
     </row>
     <row r="53" spans="4:5">
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
     </row>
     <row r="54" spans="4:5">
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
     </row>
     <row r="55" spans="4:5">
-      <c r="D55" s="12"/>
-      <c r="E55" s="18"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="14"/>
     </row>
     <row r="56" spans="4:5">
       <c r="D56" s="4"/>
@@ -1989,22 +1817,14 @@
       <c r="E91" s="4"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="H23" r:id="rId1" xr:uid="{B5EB0F45-ED5D-4DE6-9BA1-6FE6BBDD9003}"/>
-    <hyperlink ref="H10" r:id="rId2" location="packaging-material-codes" xr:uid="{6ECCDCF6-D832-47BD-BFFE-6CACBA086DC3}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="d1117845-93f6-4da3-abaa-fcb4fa669c78" ContentTypeId="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC01" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2013,7 +1833,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lae2bfa7b6474897ab4a53f76ea236c7 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
@@ -2078,7 +1898,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Defra document" ma:contentTypeID="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC01004F33776538BC6A4BB35A13B55FDEF669" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="540aecd89ea7381fdbb9d30c8a4dc936">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="662745e8-e224-48e8-a2e3-254862b8c2f5" xmlns:ns3="aa328a9d-dd77-40c9-a5eb-135ff6df47d2" xmlns:ns4="afded164-4d4a-45c5-b6a4-4c86a507a889" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f33d7f383e7ef3e5f94429c699357eeb" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2433,18 +2253,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="d1117845-93f6-4da3-abaa-fcb4fa669c78" ContentTypeId="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC01" PreviousValue="false"/>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FC065CC-1BDB-4473-8699-DD8F45A40C86}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B31069A-A18C-4C15-8712-D6A4154B76E5}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B31069A-A18C-4C15-8712-D6A4154B76E5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74398F8A-5630-46AB-8D4D-D0AED34105A4}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74398F8A-5630-46AB-8D4D-D0AED34105A4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F008D6C-356D-4A95-A106-F742FD21AA0E}"/>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F008D6C-356D-4A95-A106-F742FD21AA0E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FC065CC-1BDB-4473-8699-DD8F45A40C86}"/>
 </file>
</xml_diff>

<commit_message>
Template with changes - UD
</commit_message>
<xml_diff>
--- a/src/EPR.Calculator.Frontend/wwwroot/assets/SchemeParameterTemplates/SchemeParameterTemplate.v0.1.xlsx
+++ b/src/EPR.Calculator.Frontend/wwwroot/assets/SchemeParameterTemplates/SchemeParameterTemplate.v0.1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28005"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28007"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eviden-my.sharepoint.com/personal/chris_m_bush_eviden_com/Documents/DEFRA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CBA5ACF9-C9BF-4591-8C3F-D3824D50C444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{967CCE40-12DC-4026-9DC2-C5B695D37ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{774E54A3-E1B1-4BB4-866A-0176C4ECA77D}"/>
   </bookViews>
@@ -209,10 +209,10 @@
     <t>BADEBT-P</t>
   </si>
   <si>
-    <t>Bad debt provision percentage</t>
-  </si>
-  <si>
-    <t>BadDebt</t>
+    <t>Bad debt provision</t>
+  </si>
+  <si>
+    <t>Percentage</t>
   </si>
   <si>
     <t>MATT-AI</t>
@@ -769,8 +769,8 @@
   <dimension ref="A1:G91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22:E29"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1825,15 +1825,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lae2bfa7b6474897ab4a53f76ea236c7 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
@@ -1898,7 +1889,21 @@
 </p:properties>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="d1117845-93f6-4da3-abaa-fcb4fa669c78" ContentTypeId="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC01" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Defra document" ma:contentTypeID="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC01004F33776538BC6A4BB35A13B55FDEF669" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="540aecd89ea7381fdbb9d30c8a4dc936">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="662745e8-e224-48e8-a2e3-254862b8c2f5" xmlns:ns3="aa328a9d-dd77-40c9-a5eb-135ff6df47d2" xmlns:ns4="afded164-4d4a-45c5-b6a4-4c86a507a889" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f33d7f383e7ef3e5f94429c699357eeb" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2253,23 +2258,18 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="d1117845-93f6-4da3-abaa-fcb4fa669c78" ContentTypeId="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC01" PreviousValue="false"/>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74398F8A-5630-46AB-8D4D-D0AED34105A4}"/>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B31069A-A18C-4C15-8712-D6A4154B76E5}"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74398F8A-5630-46AB-8D4D-D0AED34105A4}"/>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F008D6C-356D-4A95-A106-F742FD21AA0E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FC065CC-1BDB-4473-8699-DD8F45A40C86}"/>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FC065CC-1BDB-4473-8699-DD8F45A40C86}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F008D6C-356D-4A95-A106-F742FD21AA0E}"/>
 </file>
</xml_diff>

<commit_message>
Template with changes - UD (#25)
</commit_message>
<xml_diff>
--- a/src/EPR.Calculator.Frontend/wwwroot/assets/SchemeParameterTemplates/SchemeParameterTemplate.v0.1.xlsx
+++ b/src/EPR.Calculator.Frontend/wwwroot/assets/SchemeParameterTemplates/SchemeParameterTemplate.v0.1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28005"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28007"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eviden-my.sharepoint.com/personal/chris_m_bush_eviden_com/Documents/DEFRA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CBA5ACF9-C9BF-4591-8C3F-D3824D50C444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{967CCE40-12DC-4026-9DC2-C5B695D37ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{774E54A3-E1B1-4BB4-866A-0176C4ECA77D}"/>
   </bookViews>
@@ -209,10 +209,10 @@
     <t>BADEBT-P</t>
   </si>
   <si>
-    <t>Bad debt provision percentage</t>
-  </si>
-  <si>
-    <t>BadDebt</t>
+    <t>Bad debt provision</t>
+  </si>
+  <si>
+    <t>Percentage</t>
   </si>
   <si>
     <t>MATT-AI</t>
@@ -769,8 +769,8 @@
   <dimension ref="A1:G91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22:E29"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1825,15 +1825,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lae2bfa7b6474897ab4a53f76ea236c7 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
@@ -1898,7 +1889,21 @@
 </p:properties>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="d1117845-93f6-4da3-abaa-fcb4fa669c78" ContentTypeId="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC01" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Defra document" ma:contentTypeID="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC01004F33776538BC6A4BB35A13B55FDEF669" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="540aecd89ea7381fdbb9d30c8a4dc936">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="662745e8-e224-48e8-a2e3-254862b8c2f5" xmlns:ns3="aa328a9d-dd77-40c9-a5eb-135ff6df47d2" xmlns:ns4="afded164-4d4a-45c5-b6a4-4c86a507a889" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f33d7f383e7ef3e5f94429c699357eeb" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2253,23 +2258,18 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="d1117845-93f6-4da3-abaa-fcb4fa669c78" ContentTypeId="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC01" PreviousValue="false"/>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74398F8A-5630-46AB-8D4D-D0AED34105A4}"/>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B31069A-A18C-4C15-8712-D6A4154B76E5}"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74398F8A-5630-46AB-8D4D-D0AED34105A4}"/>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F008D6C-356D-4A95-A106-F742FD21AA0E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FC065CC-1BDB-4473-8699-DD8F45A40C86}"/>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FC065CC-1BDB-4473-8699-DD8F45A40C86}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F008D6C-356D-4A95-A106-F742FD21AA0E}"/>
 </file>
</xml_diff>